<commit_message>
formateado a 2 decimales
</commit_message>
<xml_diff>
--- a/ReporteRankingVinos/static/vinos.xlsx
+++ b/ReporteRankingVinos/static/vinos.xlsx
@@ -12,21 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
-  <si>
-    <t>92.66666666666667</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t>Puntaje</t>
+  </si>
+  <si>
+    <t>Datos del vino</t>
+  </si>
+  <si>
+    <t>92,67</t>
   </si>
   <si>
     <t>Montes Alpha Cabernet Sauvignon - 4500.0 - Bodega Montes, Colchagua Andes, Colchagua, Chile - [Cabernet Gran Reserva]</t>
   </si>
   <si>
-    <t>92.33333333333333</t>
+    <t>92,33</t>
   </si>
   <si>
     <t>Norton Chardonnay Reserva - 3100.0 - Bodega Norton, Valle de Uco, Mendoza, Argentina - [Chardonnay Clásico]</t>
   </si>
   <si>
-    <t>91.33333333333333</t>
+    <t>91,33</t>
   </si>
   <si>
     <t>Garzón Albariño - 3800.0 - Bodega Garzón, Las Violetas, Canelones, Uruguay - [Sauvignon Blanc Finca]</t>
@@ -35,7 +41,7 @@
     <t>Norton Sauvignon Blanc - 3000.0 - Bodega Norton, Valle de Uco, Mendoza, Argentina - [Sauvignon Blanc Finca]</t>
   </si>
   <si>
-    <t>91.0</t>
+    <t>91,00</t>
   </si>
   <si>
     <t>Norton Malbec - 2900.0 - Bodega Norton, Valle de Uco, Mendoza, Argentina - [Malbec Reserva]</t>
@@ -47,7 +53,7 @@
     <t>Garzón Tannat - 4000.0 - Bodega Garzón, Las Violetas, Canelones, Uruguay - [Pinot Noir Reserva]</t>
   </si>
   <si>
-    <t>90.0</t>
+    <t>90,00</t>
   </si>
   <si>
     <t>Trapiche Malbec - 2500.0 - Bodega Trapiche, Luján de Cuyo, Mendoza, Argentina - [Malbec Reserva]</t>
@@ -64,13 +70,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,25 +104,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
     </row>
@@ -133,15 +145,15 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>8</v>
@@ -149,23 +161,23 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>12</v>
@@ -173,18 +185,26 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>